<commit_message>
work on at school
</commit_message>
<xml_diff>
--- a/res/backgrounds/bglevel.xlsx
+++ b/res/backgrounds/bglevel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krystle\Documents\GitHub\cs134netbeans\cs134\backgrounds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kori\Documents\GitHub\cs134netbeans\cs134\res\backgrounds\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,6 +23,14 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+  <si>
+    <t>C</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
@@ -34,7 +42,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -62,6 +70,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -93,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -101,6 +115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,15 +430,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BY1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="37" width="4.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5"/>
@@ -431,7 +449,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="E2" s="4"/>
       <c r="F2" s="6"/>
       <c r="G2" s="5"/>
@@ -439,7 +457,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="E3" s="4"/>
       <c r="F3" s="6"/>
       <c r="G3" s="5"/>
@@ -447,7 +465,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="5"/>
@@ -455,7 +473,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="E5" s="4"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -463,7 +481,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="E6" s="4"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -471,20 +489,15 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="T11" s="1">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="S12" s="1">
-        <v>136</v>
-      </c>
-      <c r="T12" s="3">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="I12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>68</v>
       </c>
@@ -530,23 +543,53 @@
       <c r="O13">
         <v>68</v>
       </c>
-      <c r="P13" s="1">
+      <c r="P13">
+        <v>68</v>
+      </c>
+      <c r="Q13">
+        <v>68</v>
+      </c>
+      <c r="R13">
+        <v>68</v>
+      </c>
+      <c r="S13" s="1">
         <v>142</v>
       </c>
-      <c r="Q13" s="1">
-        <v>125</v>
-      </c>
-      <c r="R13" s="1">
+      <c r="T13" s="1">
         <v>130</v>
       </c>
-      <c r="S13" s="3">
-        <v>135</v>
-      </c>
-      <c r="T13">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="1">
+        <v>106</v>
+      </c>
+      <c r="V13" s="1">
+        <v>106</v>
+      </c>
+      <c r="W13" s="1">
+        <v>151</v>
+      </c>
+      <c r="X13" s="1">
+        <v>152</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>193</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>188</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>183</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>178</v>
+      </c>
+      <c r="AG13" s="1">
+        <v>173</v>
+      </c>
+      <c r="AH13" s="1">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>68</v>
       </c>
@@ -565,26 +608,26 @@
       <c r="F14">
         <v>68</v>
       </c>
-      <c r="G14">
-        <v>68</v>
+      <c r="G14" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="H14">
         <v>68</v>
       </c>
-      <c r="I14">
-        <v>68</v>
-      </c>
-      <c r="J14">
-        <v>68</v>
+      <c r="I14" s="2">
+        <v>111</v>
+      </c>
+      <c r="J14" s="2">
+        <v>110</v>
       </c>
       <c r="K14">
         <v>68</v>
       </c>
-      <c r="L14" s="2">
-        <v>111</v>
-      </c>
-      <c r="M14" s="2">
-        <v>110</v>
+      <c r="L14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>68</v>
       </c>
       <c r="N14">
         <v>68</v>
@@ -592,23 +635,68 @@
       <c r="O14">
         <v>68</v>
       </c>
-      <c r="P14" s="1">
+      <c r="P14">
+        <v>68</v>
+      </c>
+      <c r="Q14">
+        <v>68</v>
+      </c>
+      <c r="R14">
+        <v>68</v>
+      </c>
+      <c r="S14" s="1">
         <v>141</v>
       </c>
-      <c r="Q14" s="3">
-        <v>124</v>
-      </c>
-      <c r="R14" s="3">
+      <c r="T14" s="3">
         <v>129</v>
       </c>
-      <c r="S14">
-        <v>134</v>
-      </c>
-      <c r="T14">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="3">
+        <v>121</v>
+      </c>
+      <c r="V14" s="3">
+        <v>121</v>
+      </c>
+      <c r="W14" s="3">
+        <v>150</v>
+      </c>
+      <c r="X14" s="1">
+        <v>153</v>
+      </c>
+      <c r="Z14">
+        <v>68</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>201</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>197</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>192</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>187</v>
+      </c>
+      <c r="AE14" s="3">
+        <v>182</v>
+      </c>
+      <c r="AF14" s="3">
+        <v>177</v>
+      </c>
+      <c r="AG14" s="3">
+        <v>172</v>
+      </c>
+      <c r="AH14" s="1">
+        <v>167</v>
+      </c>
+      <c r="AI14" s="1">
+        <v>163</v>
+      </c>
+      <c r="AJ14" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>106</v>
       </c>
@@ -634,43 +722,94 @@
         <v>107</v>
       </c>
       <c r="I15" s="1">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J15" s="1">
+        <v>109</v>
+      </c>
+      <c r="K15" s="1">
+        <v>106</v>
+      </c>
+      <c r="L15" s="1">
         <v>107</v>
       </c>
-      <c r="K15" s="1">
-        <v>106</v>
-      </c>
-      <c r="L15" s="1">
-        <v>108</v>
-      </c>
       <c r="M15" s="1">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="N15" s="1">
         <v>107</v>
       </c>
       <c r="O15" s="1">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="P15" s="1">
-        <v>106</v>
-      </c>
-      <c r="Q15">
-        <v>105</v>
-      </c>
-      <c r="R15">
+        <v>107</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>106</v>
+      </c>
+      <c r="R15" s="1">
+        <v>107</v>
+      </c>
+      <c r="S15" s="1">
+        <v>106</v>
+      </c>
+      <c r="T15" s="3">
         <v>128</v>
       </c>
-      <c r="S15">
+      <c r="U15" s="3">
         <v>133</v>
       </c>
-      <c r="T15">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V15" s="3">
+        <v>143</v>
+      </c>
+      <c r="W15" s="3">
+        <v>149</v>
+      </c>
+      <c r="X15" s="1">
+        <v>107</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>106</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>107</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>200</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>196</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>191</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>186</v>
+      </c>
+      <c r="AE15" s="3">
+        <v>181</v>
+      </c>
+      <c r="AF15" s="3">
+        <v>176</v>
+      </c>
+      <c r="AG15" s="3">
+        <v>171</v>
+      </c>
+      <c r="AH15" s="3">
+        <v>166</v>
+      </c>
+      <c r="AI15" s="1">
+        <v>162</v>
+      </c>
+      <c r="AJ15" s="1">
+        <v>159</v>
+      </c>
+      <c r="AK15" s="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>121</v>
       </c>
@@ -696,10 +835,10 @@
         <v>122</v>
       </c>
       <c r="I16" s="3">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J16" s="3">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K16" s="3">
         <v>121</v>
@@ -719,78 +858,278 @@
       <c r="P16" s="3">
         <v>122</v>
       </c>
-      <c r="Q16">
-        <v>121</v>
-      </c>
-      <c r="R16">
+      <c r="Q16" s="3">
+        <v>121</v>
+      </c>
+      <c r="R16" s="3">
+        <v>122</v>
+      </c>
+      <c r="S16" s="3">
+        <v>121</v>
+      </c>
+      <c r="T16" s="3">
         <v>127</v>
       </c>
-      <c r="S16">
+      <c r="U16" s="3">
         <v>132</v>
       </c>
-      <c r="T16">
+      <c r="V16" s="3">
+        <v>132</v>
+      </c>
+      <c r="W16" s="3">
+        <v>148</v>
+      </c>
+      <c r="X16" s="3">
+        <v>155</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>121</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>122</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>199</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>195</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>190</v>
+      </c>
+      <c r="AD16" s="3">
+        <v>185</v>
+      </c>
+      <c r="AE16" s="3">
+        <v>180</v>
+      </c>
+      <c r="AF16" s="3">
+        <v>175</v>
+      </c>
+      <c r="AG16" s="3">
+        <v>170</v>
+      </c>
+      <c r="AH16" s="3">
+        <v>165</v>
+      </c>
+      <c r="AI16" s="3">
+        <v>161</v>
+      </c>
+      <c r="AJ16" s="3">
+        <v>158</v>
+      </c>
+      <c r="AK16" s="3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>112</v>
+      </c>
+      <c r="B17" s="3">
+        <v>113</v>
+      </c>
+      <c r="C17" s="3">
+        <v>114</v>
+      </c>
+      <c r="D17" s="3">
+        <v>115</v>
+      </c>
+      <c r="E17" s="3">
+        <v>116</v>
+      </c>
+      <c r="F17" s="3">
+        <v>117</v>
+      </c>
+      <c r="G17" s="3">
+        <v>118</v>
+      </c>
+      <c r="H17" s="3">
+        <v>113</v>
+      </c>
+      <c r="I17" s="3">
+        <v>119</v>
+      </c>
+      <c r="J17" s="3">
+        <v>112</v>
+      </c>
+      <c r="K17" s="3">
+        <v>118</v>
+      </c>
+      <c r="L17" s="3">
+        <v>113</v>
+      </c>
+      <c r="M17" s="3">
+        <v>118</v>
+      </c>
+      <c r="N17" s="3">
+        <v>120</v>
+      </c>
+      <c r="O17" s="3">
+        <v>118</v>
+      </c>
+      <c r="P17" s="3">
+        <v>113</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>118</v>
+      </c>
+      <c r="R17" s="3">
+        <v>120</v>
+      </c>
+      <c r="S17" s="3">
+        <v>118</v>
+      </c>
+      <c r="T17" s="3">
+        <v>126</v>
+      </c>
+      <c r="U17" s="3">
+        <v>131</v>
+      </c>
+      <c r="V17" s="3">
+        <v>138</v>
+      </c>
+      <c r="W17" s="3">
+        <v>147</v>
+      </c>
+      <c r="X17" s="3">
+        <v>154</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>112</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>113</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>198</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>194</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>189</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>184</v>
+      </c>
+      <c r="AE17" s="3">
+        <v>179</v>
+      </c>
+      <c r="AF17" s="3">
+        <v>174</v>
+      </c>
+      <c r="AG17" s="3">
+        <v>169</v>
+      </c>
+      <c r="AH17" s="3">
+        <v>164</v>
+      </c>
+      <c r="AI17" s="3">
+        <v>137</v>
+      </c>
+      <c r="AJ17" s="3">
+        <v>157</v>
+      </c>
+      <c r="AK17" s="3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AG25" s="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AF26" s="1">
+        <v>136</v>
+      </c>
+      <c r="AG26" s="3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AC27" s="1">
+        <v>142</v>
+      </c>
+      <c r="AD27" s="1">
+        <v>125</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>130</v>
+      </c>
+      <c r="AF27" s="3">
+        <v>135</v>
+      </c>
+      <c r="AG27">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AC28" s="1">
+        <v>141</v>
+      </c>
+      <c r="AD28" s="3">
+        <v>124</v>
+      </c>
+      <c r="AE28" s="3">
+        <v>129</v>
+      </c>
+      <c r="AF28">
+        <v>134</v>
+      </c>
+      <c r="AG28">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AC29" s="1">
+        <v>106</v>
+      </c>
+      <c r="AD29">
+        <v>105</v>
+      </c>
+      <c r="AE29">
+        <v>128</v>
+      </c>
+      <c r="AF29">
+        <v>133</v>
+      </c>
+      <c r="AG29">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AC30" s="3">
+        <v>122</v>
+      </c>
+      <c r="AD30">
+        <v>121</v>
+      </c>
+      <c r="AE30">
+        <v>127</v>
+      </c>
+      <c r="AF30">
+        <v>132</v>
+      </c>
+      <c r="AG30">
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>112</v>
-      </c>
-      <c r="B17">
-        <v>113</v>
-      </c>
-      <c r="C17">
-        <v>114</v>
-      </c>
-      <c r="D17">
-        <v>115</v>
-      </c>
-      <c r="E17">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AC31">
         <v>116</v>
       </c>
-      <c r="F17">
-        <v>117</v>
-      </c>
-      <c r="G17">
-        <v>118</v>
-      </c>
-      <c r="H17">
-        <v>113</v>
-      </c>
-      <c r="I17">
-        <v>112</v>
-      </c>
-      <c r="J17">
-        <v>117</v>
-      </c>
-      <c r="K17">
-        <v>114</v>
-      </c>
-      <c r="L17">
-        <v>119</v>
-      </c>
-      <c r="M17">
-        <v>112</v>
-      </c>
-      <c r="N17">
+      <c r="AD31">
         <v>120</v>
       </c>
-      <c r="O17">
-        <v>120</v>
-      </c>
-      <c r="P17">
-        <v>116</v>
-      </c>
-      <c r="Q17">
-        <v>120</v>
-      </c>
-      <c r="R17">
+      <c r="AE31">
         <v>126</v>
       </c>
-      <c r="S17">
+      <c r="AF31">
         <v>131</v>
       </c>
-      <c r="T17">
+      <c r="AG31">
         <v>138</v>
       </c>
     </row>

</xml_diff>